<commit_message>
better address handling in excel
</commit_message>
<xml_diff>
--- a/excelOutput.xlsx
+++ b/excelOutput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\PracticePantherInterview\practice-panther-interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BC6814-F9E3-4B4B-9EA6-2D2B00D78A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0798558F-FDBB-4458-88C7-491B1DE5B593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="221">
   <si>
     <t>Client ID</t>
   </si>
@@ -776,7 +776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -784,15 +784,13 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
     <dxf>
       <font>
         <b val="0"/>
@@ -848,21 +846,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -903,6 +886,24 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <fill>
@@ -955,14 +956,14 @@
   </dxfs>
   <tableStyles count="2">
     <tableStyle name="Test file-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="12"/>
-      <tableStyleElement type="firstRowStripe" dxfId="11"/>
-      <tableStyleElement type="secondRowStripe" dxfId="10"/>
+      <tableStyleElement type="headerRow" dxfId="13"/>
+      <tableStyleElement type="firstRowStripe" dxfId="12"/>
+      <tableStyleElement type="secondRowStripe" dxfId="11"/>
     </tableStyle>
     <tableStyle name="expected output-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="9"/>
-      <tableStyleElement type="firstRowStripe" dxfId="8"/>
-      <tableStyleElement type="secondRowStripe" dxfId="7"/>
+      <tableStyleElement type="headerRow" dxfId="10"/>
+      <tableStyleElement type="firstRowStripe" dxfId="9"/>
+      <tableStyleElement type="secondRowStripe" dxfId="8"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1037,25 +1038,27 @@
     <tableColumn id="2" xr3:uid="{948A7A4E-471A-4CC2-A8C1-FE404E4DF9A3}" name="First Name"/>
     <tableColumn id="3" xr3:uid="{7E043604-1011-4C37-91AC-0DC8D28A599B}" name="MiddleName"/>
     <tableColumn id="4" xr3:uid="{0E79B58D-1D05-4D20-94C4-7D1445EB832C}" name="Last Name"/>
-    <tableColumn id="17" xr3:uid="{E7F8B51E-61D6-4340-BDFB-DD7376F369F8}" name="Full Name" dataDxfId="0">
+    <tableColumn id="17" xr3:uid="{E7F8B51E-61D6-4340-BDFB-DD7376F369F8}" name="Full Name" dataDxfId="7">
       <calculatedColumnFormula>TRIM(_xlfn.CONCAT(Table_14[[#This Row],[Last Name]],", ", Table_14[[#This Row],[First Name]]," ", Table_14[[#This Row],[MiddleName]]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{AE1E111D-CBC2-4074-B0BA-6D6168FFF911}" name="Company"/>
-    <tableColumn id="6" xr3:uid="{C06BF351-7962-472C-8050-BB01F656BECC}" name="Address"/>
-    <tableColumn id="18" xr3:uid="{D0C7A650-FCC9-426D-94FC-F7396F2C6E15}" name="Street1" dataDxfId="3">
-      <calculatedColumnFormula array="1">IFERROR(TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{C06BF351-7962-472C-8050-BB01F656BECC}" name="Address" dataDxfId="3">
+      <calculatedColumnFormula>TRIM(Table_1[[#This Row],[Address]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{67EC7E6E-B765-4556-9ACF-80FD860D1309}" name="Street2" dataDxfId="5">
-      <calculatedColumnFormula array="1">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</calculatedColumnFormula>
+    <tableColumn id="18" xr3:uid="{D0C7A650-FCC9-426D-94FC-F7396F2C6E15}" name="Street1" dataDxfId="5">
+      <calculatedColumnFormula array="1">IF(NOT(Table_14[[#This Row],[Address]] = ""),TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{1AC3535F-3B38-46CC-A04F-37F00A3514A4}" name="City" dataDxfId="4">
-      <calculatedColumnFormula array="1">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</calculatedColumnFormula>
+    <tableColumn id="19" xr3:uid="{67EC7E6E-B765-4556-9ACF-80FD860D1309}" name="Street2" dataDxfId="4">
+      <calculatedColumnFormula array="1">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{4063A8D7-2348-425E-AF64-FFF603A2B834}" name="State" dataDxfId="2">
-      <calculatedColumnFormula array="1">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</calculatedColumnFormula>
+    <tableColumn id="20" xr3:uid="{1AC3535F-3B38-46CC-A04F-37F00A3514A4}" name="City" dataDxfId="2">
+      <calculatedColumnFormula array="1">IF(NOT(Table_14[[#This Row],[Address]] = ""),IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{CB2AB3F9-D677-47EB-989D-1AB674D8D5CA}" name="Zip" dataDxfId="1">
-      <calculatedColumnFormula array="1">IFERROR(_xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</calculatedColumnFormula>
+    <tableColumn id="21" xr3:uid="{4063A8D7-2348-425E-AF64-FFF603A2B834}" name="State" dataDxfId="1">
+      <calculatedColumnFormula array="1">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="22" xr3:uid="{CB2AB3F9-D677-47EB-989D-1AB674D8D5CA}" name="Zip" dataDxfId="0">
+      <calculatedColumnFormula array="1">IF(NOT(Table_14[[#This Row],[Address]] = ""), _xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{A9B89DC4-9B9A-42F1-AD97-3520AD990342}" name="Home Fax"/>
     <tableColumn id="8" xr3:uid="{8A57D9E6-A1B8-4236-9E89-DA71E75FC139}" name="Mobile Phone"/>
@@ -5095,8 +5098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAEE9291-F283-4E21-B500-30695527D53B}">
   <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5143,19 +5146,19 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" t="s">
         <v>126</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" t="s">
         <v>127</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" t="s">
         <v>128</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" t="s">
         <v>129</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" t="s">
         <v>220</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -5207,25 +5210,28 @@
         <v>Barretta, William Tim</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="7"/>
+      <c r="G2" s="8" t="str">
+        <f>TRIM(Table_1[[#This Row],[Address]])</f>
+        <v/>
+      </c>
       <c r="H2" s="1" t="str" cm="1">
-        <f t="array" ref="H2">IFERROR(TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
+        <f t="array" ref="H2">IF(NOT(Table_14[[#This Row],[Address]] = ""),TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
         <v/>
       </c>
       <c r="I2" s="1" t="str" cm="1">
-        <f t="array" ref="I2">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
+        <f t="array" ref="I2">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
         <v/>
       </c>
       <c r="J2" s="1" t="str" cm="1">
-        <f t="array" ref="J2">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
+        <f t="array" ref="J2">IF(NOT(Table_14[[#This Row],[Address]] = ""),IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
         <v/>
       </c>
       <c r="K2" s="1" t="str" cm="1">
-        <f t="array" ref="K2">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
+        <f t="array" ref="K2">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
         <v/>
       </c>
       <c r="L2" s="1" t="str" cm="1">
-        <f t="array" ref="L2">IFERROR(_xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
+        <f t="array" ref="L2">IF(NOT(Table_14[[#This Row],[Address]] = ""), _xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
         <v/>
       </c>
       <c r="M2" s="1"/>
@@ -5264,27 +5270,28 @@
         <v>Kamel, Khaled Kayne</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
-        <v>25</v>
+      <c r="G3" s="1" t="str">
+        <f>TRIM(Table_1[[#This Row],[Address]])</f>
+        <v>2926 N Raine Blvd. 6, Tucson, State 1 11111</v>
       </c>
       <c r="H3" s="1" t="str" cm="1">
-        <f t="array" ref="H3">IFERROR(TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
+        <f t="array" ref="H3">IF(NOT(Table_14[[#This Row],[Address]] = ""),TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
         <v>2926 N Raine</v>
       </c>
       <c r="I3" s="1" t="str" cm="1">
-        <f t="array" ref="I3">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
+        <f t="array" ref="I3">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
         <v>Blvd. 6</v>
       </c>
       <c r="J3" s="1" t="str" cm="1">
-        <f t="array" ref="J3">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
+        <f t="array" ref="J3">IF(NOT(Table_14[[#This Row],[Address]] = ""),IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
         <v>Tucson</v>
       </c>
-      <c r="K3" s="8" t="str" cm="1">
-        <f t="array" ref="K3">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
+      <c r="K3" t="str" cm="1">
+        <f t="array" ref="K3">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
         <v>State 1</v>
       </c>
       <c r="L3" s="1" t="str" cm="1">
-        <f t="array" ref="L3">IFERROR(_xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
+        <f t="array" ref="L3">IF(NOT(Table_14[[#This Row],[Address]] = ""), _xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
         <v xml:space="preserve"> 11111</v>
       </c>
       <c r="M3" s="1"/>
@@ -5327,27 +5334,28 @@
         <v>Tembo, Dumisani</v>
       </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="1" t="s">
-        <v>19</v>
+      <c r="G4" s="1" t="str">
+        <f>TRIM(Table_1[[#This Row],[Address]])</f>
+        <v/>
       </c>
       <c r="H4" s="1" t="str" cm="1">
-        <f t="array" ref="H4">IFERROR(TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
+        <f t="array" ref="H4">IF(NOT(Table_14[[#This Row],[Address]] = ""),TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
         <v/>
       </c>
       <c r="I4" s="1" t="str" cm="1">
-        <f t="array" ref="I4">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
+        <f t="array" ref="I4">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
         <v/>
       </c>
       <c r="J4" s="1" t="str" cm="1">
-        <f t="array" ref="J4">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
+        <f t="array" ref="J4">IF(NOT(Table_14[[#This Row],[Address]] = ""),IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
         <v/>
       </c>
       <c r="K4" s="1" t="str" cm="1">
-        <f t="array" ref="K4">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
+        <f t="array" ref="K4">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
         <v/>
       </c>
       <c r="L4" s="1" t="str" cm="1">
-        <f t="array" ref="L4">IFERROR(_xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
+        <f t="array" ref="L4">IF(NOT(Table_14[[#This Row],[Address]] = ""), _xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
         <v/>
       </c>
       <c r="M4" s="1"/>
@@ -5388,27 +5396,28 @@
         <v>Dao, Khanh Dee</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
-        <v>36</v>
+      <c r="G5" s="1" t="str">
+        <f>TRIM(Table_1[[#This Row],[Address]])</f>
+        <v>435 N. Congress Ave., #180, St Petersburg, State 2 11111</v>
       </c>
       <c r="H5" s="1" t="str" cm="1">
-        <f t="array" ref="H5">IFERROR(TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
+        <f t="array" ref="H5">IF(NOT(Table_14[[#This Row],[Address]] = ""),TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
         <v>435 N. Congress Ave.</v>
       </c>
       <c r="I5" s="1" t="str" cm="1">
-        <f t="array" ref="I5">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
+        <f t="array" ref="I5">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
         <v>#180</v>
       </c>
       <c r="J5" s="1" t="str" cm="1">
-        <f t="array" ref="J5">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
+        <f t="array" ref="J5">IF(NOT(Table_14[[#This Row],[Address]] = ""),IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
         <v>St Petersburg</v>
       </c>
       <c r="K5" s="1" t="str" cm="1">
-        <f t="array" ref="K5">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
+        <f t="array" ref="K5">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
         <v>State 2</v>
       </c>
       <c r="L5" s="1" t="str" cm="1">
-        <f t="array" ref="L5">IFERROR(_xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
+        <f t="array" ref="L5">IF(NOT(Table_14[[#This Row],[Address]] = ""), _xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
         <v xml:space="preserve"> 11111</v>
       </c>
       <c r="M5" s="1"/>
@@ -5449,27 +5458,28 @@
         <v>Saad, Anmar</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="1" t="s">
-        <v>42</v>
+      <c r="G6" s="1" t="str">
+        <f>TRIM(Table_1[[#This Row],[Address]])</f>
+        <v>1234 Highland Square Lane, Denver, State 3 11111</v>
       </c>
       <c r="H6" s="1" t="str" cm="1">
-        <f t="array" ref="H6">IFERROR(TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
+        <f t="array" ref="H6">IF(NOT(Table_14[[#This Row],[Address]] = ""),TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
         <v>1234 Highland Square Lane</v>
       </c>
       <c r="I6" s="1" t="str" cm="1">
-        <f t="array" ref="I6">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
+        <f t="array" ref="I6">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
         <v/>
       </c>
       <c r="J6" s="1" t="str" cm="1">
-        <f t="array" ref="J6">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
+        <f t="array" ref="J6">IF(NOT(Table_14[[#This Row],[Address]] = ""),IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
         <v>Denver</v>
       </c>
       <c r="K6" s="1" t="str" cm="1">
-        <f t="array" ref="K6">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
+        <f t="array" ref="K6">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
         <v>State 3</v>
       </c>
       <c r="L6" s="1" t="str" cm="1">
-        <f t="array" ref="L6">IFERROR(_xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
+        <f t="array" ref="L6">IF(NOT(Table_14[[#This Row],[Address]] = ""), _xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
         <v xml:space="preserve"> 11111</v>
       </c>
       <c r="M6" s="1"/>
@@ -5514,27 +5524,28 @@
         <v>Colonnese, Victor Henry</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
-        <v>49</v>
+      <c r="G7" s="1" t="str">
+        <f>TRIM(Table_1[[#This Row],[Address]])</f>
+        <v>PO Box 200059, Hollywood, State 4 11111</v>
       </c>
       <c r="H7" s="1" t="str" cm="1">
-        <f t="array" ref="H7">IFERROR(TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
+        <f t="array" ref="H7">IF(NOT(Table_14[[#This Row],[Address]] = ""),TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
         <v>PO Box 200059</v>
       </c>
       <c r="I7" s="1" t="str" cm="1">
-        <f t="array" ref="I7">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
+        <f t="array" ref="I7">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
         <v/>
       </c>
       <c r="J7" s="1" t="str" cm="1">
-        <f t="array" ref="J7">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
+        <f t="array" ref="J7">IF(NOT(Table_14[[#This Row],[Address]] = ""),IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
         <v>Hollywood</v>
       </c>
       <c r="K7" s="1" t="str" cm="1">
-        <f t="array" ref="K7">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
+        <f t="array" ref="K7">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
         <v>State 4</v>
       </c>
       <c r="L7" s="1" t="str" cm="1">
-        <f t="array" ref="L7">IFERROR(_xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
+        <f t="array" ref="L7">IF(NOT(Table_14[[#This Row],[Address]] = ""), _xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
         <v xml:space="preserve"> 11111</v>
       </c>
       <c r="M7" s="1"/>
@@ -5575,27 +5586,28 @@
         <v>Hardikar, Amol</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="1" t="s">
-        <v>55</v>
+      <c r="G8" s="1" t="str">
+        <f>TRIM(Table_1[[#This Row],[Address]])</f>
+        <v>200 Perry Street, Apt. 1505, Dallas, State 5 11111</v>
       </c>
       <c r="H8" s="1" t="str" cm="1">
-        <f t="array" ref="H8">IFERROR(TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
+        <f t="array" ref="H8">IF(NOT(Table_14[[#This Row],[Address]] = ""),TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
         <v>200 Perry Street</v>
       </c>
       <c r="I8" s="1" t="str" cm="1">
-        <f t="array" ref="I8">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
+        <f t="array" ref="I8">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
         <v>Apt. 1505</v>
       </c>
       <c r="J8" s="1" t="str" cm="1">
-        <f t="array" ref="J8">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
+        <f t="array" ref="J8">IF(NOT(Table_14[[#This Row],[Address]] = ""),IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
         <v>Dallas</v>
       </c>
       <c r="K8" s="1" t="str" cm="1">
-        <f t="array" ref="K8">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
+        <f t="array" ref="K8">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
         <v>State 5</v>
       </c>
       <c r="L8" s="1" t="str" cm="1">
-        <f t="array" ref="L8">IFERROR(_xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
+        <f t="array" ref="L8">IF(NOT(Table_14[[#This Row],[Address]] = ""), _xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
         <v xml:space="preserve"> 11111</v>
       </c>
       <c r="M8" s="1"/>
@@ -5636,27 +5648,28 @@
         <v>Tachtook, Tacktook</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="1" t="s">
-        <v>61</v>
+      <c r="G9" s="1" t="str">
+        <f>TRIM(Table_1[[#This Row],[Address]])</f>
+        <v>20 Barry Court Apt 203, Boston, State 6 11111</v>
       </c>
       <c r="H9" s="1" t="str" cm="1">
-        <f t="array" ref="H9">IFERROR(TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
+        <f t="array" ref="H9">IF(NOT(Table_14[[#This Row],[Address]] = ""),TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
         <v>20 Barry Court</v>
       </c>
       <c r="I9" s="1" t="str" cm="1">
-        <f t="array" ref="I9">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
+        <f t="array" ref="I9">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
         <v>Apt 203</v>
       </c>
       <c r="J9" s="1" t="str" cm="1">
-        <f t="array" ref="J9">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
+        <f t="array" ref="J9">IF(NOT(Table_14[[#This Row],[Address]] = ""),IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
         <v>Boston</v>
       </c>
       <c r="K9" s="1" t="str" cm="1">
-        <f t="array" ref="K9">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
+        <f t="array" ref="K9">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
         <v>State 6</v>
       </c>
       <c r="L9" s="1" t="str" cm="1">
-        <f t="array" ref="L9">IFERROR(_xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
+        <f t="array" ref="L9">IF(NOT(Table_14[[#This Row],[Address]] = ""), _xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
         <v xml:space="preserve"> 11111</v>
       </c>
       <c r="M9" s="1"/>
@@ -5697,27 +5710,28 @@
         <v>Doe, John</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="1" t="s">
-        <v>67</v>
+      <c r="G10" s="1" t="str">
+        <f>TRIM(Table_1[[#This Row],[Address]])</f>
+        <v>123 Main St., Santa Ana, State 7 11111</v>
       </c>
       <c r="H10" s="1" t="str" cm="1">
-        <f t="array" ref="H10">IFERROR(TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
+        <f t="array" ref="H10">IF(NOT(Table_14[[#This Row],[Address]] = ""),TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
         <v>123 Main St.</v>
       </c>
       <c r="I10" s="1" t="str" cm="1">
-        <f t="array" ref="I10">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
+        <f t="array" ref="I10">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
         <v/>
       </c>
       <c r="J10" s="1" t="str" cm="1">
-        <f t="array" ref="J10">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
+        <f t="array" ref="J10">IF(NOT(Table_14[[#This Row],[Address]] = ""),IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
         <v>Santa Ana</v>
       </c>
       <c r="K10" s="1" t="str" cm="1">
-        <f t="array" ref="K10">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
+        <f t="array" ref="K10">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
         <v>State 7</v>
       </c>
       <c r="L10" s="1" t="str" cm="1">
-        <f t="array" ref="L10">IFERROR(_xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
+        <f t="array" ref="L10">IF(NOT(Table_14[[#This Row],[Address]] = ""), _xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
         <v xml:space="preserve"> 11111</v>
       </c>
       <c r="M10" s="1"/>
@@ -5758,27 +5772,28 @@
         <v>Nishimata, Marjorie</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="1" t="s">
-        <v>73</v>
+      <c r="G11" s="1" t="str">
+        <f>TRIM(Table_1[[#This Row],[Address]])</f>
+        <v>223 Greaterwealth Avenue Unit 70, Davie, State 8 11111</v>
       </c>
       <c r="H11" s="1" t="str" cm="1">
-        <f t="array" ref="H11">IFERROR(TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
+        <f t="array" ref="H11">IF(NOT(Table_14[[#This Row],[Address]] = ""),TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
         <v>223 Greaterwealth Avenue</v>
       </c>
       <c r="I11" s="1" t="str" cm="1">
-        <f t="array" ref="I11">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
+        <f t="array" ref="I11">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
         <v>Unit 70</v>
       </c>
       <c r="J11" s="1" t="str" cm="1">
-        <f t="array" ref="J11">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
+        <f t="array" ref="J11">IF(NOT(Table_14[[#This Row],[Address]] = ""),IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
         <v>Davie</v>
       </c>
       <c r="K11" s="1" t="str" cm="1">
-        <f t="array" ref="K11">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
+        <f t="array" ref="K11">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
         <v>State 8</v>
       </c>
       <c r="L11" s="1" t="str" cm="1">
-        <f t="array" ref="L11">IFERROR(_xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
+        <f t="array" ref="L11">IF(NOT(Table_14[[#This Row],[Address]] = ""), _xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
         <v xml:space="preserve"> 11111</v>
       </c>
       <c r="M11" s="1"/>
@@ -5821,27 +5836,28 @@
         <v>Fayad, Hamdy</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="1" t="s">
-        <v>79</v>
+      <c r="G12" s="1" t="str">
+        <f>TRIM(Table_1[[#This Row],[Address]])</f>
+        <v>2036 Bryan Street, Houston, State 9 11111</v>
       </c>
       <c r="H12" s="1" t="str" cm="1">
-        <f t="array" ref="H12">IFERROR(TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
+        <f t="array" ref="H12">IF(NOT(Table_14[[#This Row],[Address]] = ""),TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
         <v>2036 Bryan Street</v>
       </c>
       <c r="I12" s="1" t="str" cm="1">
-        <f t="array" ref="I12">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
+        <f t="array" ref="I12">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
         <v/>
       </c>
       <c r="J12" s="1" t="str" cm="1">
-        <f t="array" ref="J12">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
+        <f t="array" ref="J12">IF(NOT(Table_14[[#This Row],[Address]] = ""),IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
         <v>Houston</v>
       </c>
       <c r="K12" s="1" t="str" cm="1">
-        <f t="array" ref="K12">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
+        <f t="array" ref="K12">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
         <v>State 9</v>
       </c>
       <c r="L12" s="1" t="str" cm="1">
-        <f t="array" ref="L12">IFERROR(_xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
+        <f t="array" ref="L12">IF(NOT(Table_14[[#This Row],[Address]] = ""), _xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
         <v xml:space="preserve"> 11111</v>
       </c>
       <c r="M12" s="1"/>
@@ -5884,27 +5900,28 @@
         <v>Hersey, Jaime Lee</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="1" t="s">
-        <v>85</v>
+      <c r="G13" s="1" t="str">
+        <f>TRIM(Table_1[[#This Row],[Address]])</f>
+        <v>99 W 10th Avenue Unit 14D, Flint, State 10 11111</v>
       </c>
       <c r="H13" s="1" t="str" cm="1">
-        <f t="array" ref="H13">IFERROR(TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
+        <f t="array" ref="H13">IF(NOT(Table_14[[#This Row],[Address]] = ""),TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
         <v>99 W 10th Avenue</v>
       </c>
       <c r="I13" s="1" t="str" cm="1">
-        <f t="array" ref="I13">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
+        <f t="array" ref="I13">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
         <v>Unit 14D</v>
       </c>
       <c r="J13" s="1" t="str" cm="1">
-        <f t="array" ref="J13">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
+        <f t="array" ref="J13">IF(NOT(Table_14[[#This Row],[Address]] = ""),IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
         <v>Flint</v>
       </c>
       <c r="K13" s="1" t="str" cm="1">
-        <f t="array" ref="K13">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
+        <f t="array" ref="K13">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
         <v>State 10</v>
       </c>
       <c r="L13" s="1" t="str" cm="1">
-        <f t="array" ref="L13">IFERROR(_xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
+        <f t="array" ref="L13">IF(NOT(Table_14[[#This Row],[Address]] = ""), _xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
         <v xml:space="preserve"> 11111</v>
       </c>
       <c r="M13" s="1"/>
@@ -5949,27 +5966,28 @@
         <v>Valencia, Andrew Rosete</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="1" t="s">
-        <v>91</v>
+      <c r="G14" s="1" t="str">
+        <f>TRIM(Table_1[[#This Row],[Address]])</f>
+        <v>100 Hylein, Unit 4, Tampa, State 11 11111</v>
       </c>
       <c r="H14" s="1" t="str" cm="1">
-        <f t="array" ref="H14">IFERROR(TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
+        <f t="array" ref="H14">IF(NOT(Table_14[[#This Row],[Address]] = ""),TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
         <v>100 Hylein</v>
       </c>
       <c r="I14" s="1" t="str" cm="1">
-        <f t="array" ref="I14">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
+        <f t="array" ref="I14">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
         <v>Unit 4</v>
       </c>
       <c r="J14" s="1" t="str" cm="1">
-        <f t="array" ref="J14">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
+        <f t="array" ref="J14">IF(NOT(Table_14[[#This Row],[Address]] = ""),IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
         <v>Tampa</v>
       </c>
       <c r="K14" s="1" t="str" cm="1">
-        <f t="array" ref="K14">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
+        <f t="array" ref="K14">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
         <v>State 11</v>
       </c>
       <c r="L14" s="1" t="str" cm="1">
-        <f t="array" ref="L14">IFERROR(_xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
+        <f t="array" ref="L14">IF(NOT(Table_14[[#This Row],[Address]] = ""), _xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
         <v xml:space="preserve"> 11111</v>
       </c>
       <c r="M14" s="1"/>
@@ -6010,27 +6028,28 @@
         <v>Hou, Yen-Ming</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="1" t="s">
-        <v>97</v>
+      <c r="G15" s="1" t="str">
+        <f>TRIM(Table_1[[#This Row],[Address]])</f>
+        <v>901 Skycreek Drive #87, Miami, State 12 11111</v>
       </c>
       <c r="H15" s="1" t="str" cm="1">
-        <f t="array" ref="H15">IFERROR(TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
+        <f t="array" ref="H15">IF(NOT(Table_14[[#This Row],[Address]] = ""),TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
         <v>901 Skycreek Drive</v>
       </c>
       <c r="I15" s="1" t="str" cm="1">
-        <f t="array" ref="I15">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
+        <f t="array" ref="I15">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
         <v>#87</v>
       </c>
       <c r="J15" s="1" t="str" cm="1">
-        <f t="array" ref="J15">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
+        <f t="array" ref="J15">IF(NOT(Table_14[[#This Row],[Address]] = ""),IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
         <v>Miami</v>
       </c>
       <c r="K15" s="1" t="str" cm="1">
-        <f t="array" ref="K15">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
+        <f t="array" ref="K15">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
         <v>State 12</v>
       </c>
       <c r="L15" s="1" t="str" cm="1">
-        <f t="array" ref="L15">IFERROR(_xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
+        <f t="array" ref="L15">IF(NOT(Table_14[[#This Row],[Address]] = ""), _xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
         <v xml:space="preserve"> 11111</v>
       </c>
       <c r="M15" s="1"/>
@@ -6073,27 +6092,28 @@
         <v>Bryant, Matthew Phil</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="1" t="s">
-        <v>104</v>
+      <c r="G16" s="1" t="str">
+        <f>TRIM(Table_1[[#This Row],[Address]])</f>
+        <v>4009 Bayle Street, Apt 803, Seattle, State 13 11111</v>
       </c>
       <c r="H16" s="1" t="str" cm="1">
-        <f t="array" ref="H16">IFERROR(TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
+        <f t="array" ref="H16">IF(NOT(Table_14[[#This Row],[Address]] = ""),TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
         <v>4009 Bayle Street</v>
       </c>
       <c r="I16" s="1" t="str" cm="1">
-        <f t="array" ref="I16">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
+        <f t="array" ref="I16">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
         <v>Apt 803</v>
       </c>
       <c r="J16" s="1" t="str" cm="1">
-        <f t="array" ref="J16">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
+        <f t="array" ref="J16">IF(NOT(Table_14[[#This Row],[Address]] = ""),IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
         <v>Seattle</v>
       </c>
       <c r="K16" s="1" t="str" cm="1">
-        <f t="array" ref="K16">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
+        <f t="array" ref="K16">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
         <v>State 13</v>
       </c>
       <c r="L16" s="1" t="str" cm="1">
-        <f t="array" ref="L16">IFERROR(_xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
+        <f t="array" ref="L16">IF(NOT(Table_14[[#This Row],[Address]] = ""), _xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
         <v xml:space="preserve"> 11111</v>
       </c>
       <c r="M16" s="1"/>
@@ -6136,27 +6156,28 @@
         <v>Scanlan, Brittany Christine</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="1" t="s">
-        <v>110</v>
+      <c r="G17" s="1" t="str">
+        <f>TRIM(Table_1[[#This Row],[Address]])</f>
+        <v>101 Boardway Ave., Apt.#21, Fort Lauderdale, State 14 11111</v>
       </c>
       <c r="H17" s="1" t="str" cm="1">
-        <f t="array" ref="H17">IFERROR(TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
+        <f t="array" ref="H17">IF(NOT(Table_14[[#This Row],[Address]] = ""),TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
         <v>101 Boardway Ave.</v>
       </c>
       <c r="I17" s="1" t="str" cm="1">
-        <f t="array" ref="I17">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
+        <f t="array" ref="I17">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
         <v>Apt.#21</v>
       </c>
       <c r="J17" s="1" t="str" cm="1">
-        <f t="array" ref="J17">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
+        <f t="array" ref="J17">IF(NOT(Table_14[[#This Row],[Address]] = ""),IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
         <v>Fort Lauderdale</v>
       </c>
       <c r="K17" s="1" t="str" cm="1">
-        <f t="array" ref="K17">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
+        <f t="array" ref="K17">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
         <v>State 14</v>
       </c>
       <c r="L17" s="1" t="str" cm="1">
-        <f t="array" ref="L17">IFERROR(_xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
+        <f t="array" ref="L17">IF(NOT(Table_14[[#This Row],[Address]] = ""), _xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
         <v xml:space="preserve"> 11111</v>
       </c>
       <c r="M17" s="1"/>
@@ -6197,27 +6218,28 @@
         <v>Gotelli, Lauren</v>
       </c>
       <c r="F18" s="1"/>
-      <c r="G18" s="1" t="s">
-        <v>116</v>
+      <c r="G18" s="1" t="str">
+        <f>TRIM(Table_1[[#This Row],[Address]])</f>
+        <v>6078 Burneigh Ave., #3, Orlando, State 15 11111</v>
       </c>
       <c r="H18" s="1" t="str" cm="1">
-        <f t="array" ref="H18">IFERROR(TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
+        <f t="array" ref="H18">IF(NOT(Table_14[[#This Row],[Address]] = ""),TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
         <v>6078 Burneigh Ave.</v>
       </c>
       <c r="I18" s="1" t="str" cm="1">
-        <f t="array" ref="I18">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
+        <f t="array" ref="I18">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
         <v>#3</v>
       </c>
       <c r="J18" s="1" t="str" cm="1">
-        <f t="array" ref="J18">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
+        <f t="array" ref="J18">IF(NOT(Table_14[[#This Row],[Address]] = ""),IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
         <v>Orlando</v>
       </c>
       <c r="K18" s="1" t="str" cm="1">
-        <f t="array" ref="K18">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
+        <f t="array" ref="K18">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
         <v>State 15</v>
       </c>
       <c r="L18" s="1" t="str" cm="1">
-        <f t="array" ref="L18">IFERROR(_xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
+        <f t="array" ref="L18">IF(NOT(Table_14[[#This Row],[Address]] = ""), _xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
         <v xml:space="preserve"> 11111</v>
       </c>
       <c r="M18" s="1"/>
@@ -6260,27 +6282,28 @@
         <v>Gutierrez, Margarita</v>
       </c>
       <c r="F19" s="1"/>
-      <c r="G19" s="1" t="s">
-        <v>122</v>
+      <c r="G19" s="1" t="str">
+        <f>TRIM(Table_1[[#This Row],[Address]])</f>
+        <v>9087 Christmas Drive # 101, Las Vegas, State 16 11111</v>
       </c>
       <c r="H19" s="1" t="str" cm="1">
-        <f t="array" ref="H19">IFERROR(TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
+        <f t="array" ref="H19">IF(NOT(Table_14[[#This Row],[Address]] = ""),TRIM(IF(AND(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, Table_14[[#This Row],[Street2]]), _xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1), Table_14[[#This Row],[Street2]], ""), _xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1))), "")</f>
         <v>9087 Christmas Drive</v>
       </c>
       <c r="I19" s="1" t="str" cm="1">
-        <f t="array" ref="I19">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
+        <f t="array" ref="I19">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, IFERROR(_xlfn.REGEXEXTRACT(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),1),"(unit|apt|apartment|#|blvd)\.?\s?\w*$",,1), ""), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2))), "")</f>
         <v># 101</v>
       </c>
       <c r="J19" s="1" t="str" cm="1">
-        <f t="array" ref="J19">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
+        <f t="array" ref="J19">IF(NOT(Table_14[[#This Row],[Address]] = ""),IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),2)), TRIM(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3))), "")</f>
         <v>Las Vegas</v>
       </c>
       <c r="K19" s="1" t="str" cm="1">
-        <f t="array" ref="K19">IFERROR(IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
+        <f t="array" ref="K19">IF(NOT(Table_14[[#This Row],[Address]] = ""), IF(COUNTA(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","))=3, TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),3),Table_14[[#This Row],[Zip]],"")), TRIM(_xlfn.REGEXREPLACE(_xlfn.CHOOSECOLS(_xlfn.TEXTSPLIT(Table_14[[#This Row],[Address]],","),4),Table_14[[#This Row],[Zip]],""))), "")</f>
         <v>State 16</v>
       </c>
       <c r="L19" s="1" t="str" cm="1">
-        <f t="array" ref="L19">IFERROR(_xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
+        <f t="array" ref="L19">IF(NOT(Table_14[[#This Row],[Address]] = ""), _xlfn.REGEXEXTRACT(TRIM(Table_14[[#This Row],[Address]]),"\s[0-9]{5}(-[0-9]{4})?$"), "")</f>
         <v xml:space="preserve"> 11111</v>
       </c>
       <c r="M19" s="1"/>
@@ -6304,7 +6327,7 @@
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="H23" s="10"/>
+      <c r="H23" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>